<commit_message>
feat: Added logging to the start and end of activities also raise warning when result not found
</commit_message>
<xml_diff>
--- a/company_list.xlsx
+++ b/company_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nling\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wayne\OneDrive\桌面\infosys300\Project-6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEFE552-1F62-4CEA-9189-7B5AD47E32A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FE7865-2A5B-4423-AB0C-559F915B0B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{555E44EB-3A74-440F-909F-32CDD2B4A824}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{555E44EB-3A74-440F-909F-32CDD2B4A824}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,115 +478,115 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.88671875" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
feat: Fixed error handling for exceeding rate limit, set output excel template,added time recorded column, shifted incorporation date extraction to companies office, created a report sheet.
</commit_message>
<xml_diff>
--- a/company_list.xlsx
+++ b/company_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nling\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wayne\OneDrive\桌面\project - 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEFE552-1F62-4CEA-9189-7B5AD47E32A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B4C9DA-5612-425B-9A11-E004FA61351E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{555E44EB-3A74-440F-909F-32CDD2B4A824}"/>
+    <workbookView xWindow="1590" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{555E44EB-3A74-440F-909F-32CDD2B4A824}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,12 @@
     <t>Scenario 1 List of Companies</t>
   </si>
   <si>
+    <t>ELEPHANT FEATHER LIMITED</t>
+  </si>
+  <si>
+    <t>BAT VENTURES LIMITED</t>
+  </si>
+  <si>
     <t>CAT DOCTOR LIMITED</t>
   </si>
   <si>
@@ -62,10 +68,7 @@
     <t>FISH ENTERTAINMENT LIMITED</t>
   </si>
   <si>
-    <t>ELEPHANT FEATHER LIMITED</t>
-  </si>
-  <si>
-    <t>BAT VENTURES LIMITED</t>
+    <t>GERBIL FEEDING LIMITED</t>
   </si>
   <si>
     <t>SEAL HOUSE LIMITED </t>
@@ -74,6 +77,9 @@
     <t>SHARK WEEK LIMITED</t>
   </si>
   <si>
+    <t>WHALE VENTURES LIMITED</t>
+  </si>
+  <si>
     <t>OCTOPUS MOTORS LIMITED</t>
   </si>
   <si>
@@ -87,12 +93,6 @@
   </si>
   <si>
     <t>CHICKEN MADNESS LIMITED</t>
-  </si>
-  <si>
-    <t>GERBIL FEEDING LIMITED</t>
-  </si>
-  <si>
-    <t>WHALE VENTURES LIMITED</t>
   </si>
   <si>
     <t>CROW PIES LIMITED</t>
@@ -478,115 +478,115 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.88671875" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
feat: Fixed opencorporates scraper bug
</commit_message>
<xml_diff>
--- a/company_list.xlsx
+++ b/company_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wayne\OneDrive\桌面\project - 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B4C9DA-5612-425B-9A11-E004FA61351E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1333768E-60A7-49B5-8564-5267B7668E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1590" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{555E44EB-3A74-440F-909F-32CDD2B4A824}"/>
   </bookViews>
@@ -44,58 +44,58 @@
     <t>BAT VENTURES LIMITED</t>
   </si>
   <si>
+    <t>DOG BLOG LIMITED</t>
+  </si>
+  <si>
+    <t>RABBIT ENTERPRISES LIMITED</t>
+  </si>
+  <si>
+    <t>RAT WASH LIMITED</t>
+  </si>
+  <si>
+    <t>BIRD CALLS LIMITED</t>
+  </si>
+  <si>
+    <t>HAMSTER RENTALS LIMITED</t>
+  </si>
+  <si>
+    <t>TURTLE FARMING LIMITED</t>
+  </si>
+  <si>
+    <t>FISH ENTERTAINMENT LIMITED</t>
+  </si>
+  <si>
+    <t>GERBIL FEEDING LIMITED</t>
+  </si>
+  <si>
+    <t>SEAL HOUSE LIMITED </t>
+  </si>
+  <si>
+    <t>SHARK WEEK LIMITED</t>
+  </si>
+  <si>
+    <t>WHALE VENTURES LIMITED</t>
+  </si>
+  <si>
+    <t>OCTOPUS MOTORS LIMITED</t>
+  </si>
+  <si>
+    <t>PIG FLATS WINE COMPANY LIMITED</t>
+  </si>
+  <si>
+    <t>LAMB AG LIMITED</t>
+  </si>
+  <si>
+    <t>DUCK DUDE LIMITED</t>
+  </si>
+  <si>
+    <t>CHICKEN MADNESS LIMITED</t>
+  </si>
+  <si>
+    <t>CROW PIES LIMITED</t>
+  </si>
+  <si>
     <t>CAT DOCTOR LIMITED</t>
-  </si>
-  <si>
-    <t>DOG BLOG LIMITED</t>
-  </si>
-  <si>
-    <t>RABBIT ENTERPRISES LIMITED</t>
-  </si>
-  <si>
-    <t>RAT WASH LIMITED</t>
-  </si>
-  <si>
-    <t>BIRD CALLS LIMITED</t>
-  </si>
-  <si>
-    <t>HAMSTER RENTALS LIMITED</t>
-  </si>
-  <si>
-    <t>TURTLE FARMING LIMITED</t>
-  </si>
-  <si>
-    <t>FISH ENTERTAINMENT LIMITED</t>
-  </si>
-  <si>
-    <t>GERBIL FEEDING LIMITED</t>
-  </si>
-  <si>
-    <t>SEAL HOUSE LIMITED </t>
-  </si>
-  <si>
-    <t>SHARK WEEK LIMITED</t>
-  </si>
-  <si>
-    <t>WHALE VENTURES LIMITED</t>
-  </si>
-  <si>
-    <t>OCTOPUS MOTORS LIMITED</t>
-  </si>
-  <si>
-    <t>PIG FLATS WINE COMPANY LIMITED</t>
-  </si>
-  <si>
-    <t>LAMB AG LIMITED</t>
-  </si>
-  <si>
-    <t>DUCK DUDE LIMITED</t>
-  </si>
-  <si>
-    <t>CHICKEN MADNESS LIMITED</t>
-  </si>
-  <si>
-    <t>CROW PIES LIMITED</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,47 +493,47 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -548,47 +548,47 @@
     </row>
     <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>